<commit_message>
(XF-488) - Modified ObjectRepository.XFormDashboard - Change the previous cssSelectors of XFormDashboard - Added a function to use the main menu options with HashMap in XFormDashboard - Changed name of one Enum to match the others - Added actions.MainMenuActions to be used with the XFormDashboard - Added wait for element text to common - Added more title to enum.BodyTitles
Signed-off-by: josue-martinez-jd <josue.martinez@janeirodigital.com>
</commit_message>
<xml_diff>
--- a/xform-automation-webdriver/controllers/src/main/resources/ParameterFile.xlsx
+++ b/xform-automation-webdriver/controllers/src/main/resources/ParameterFile.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Profiles" sheetId="1" r:id="rId1"/>
     <sheet name="Parameters" sheetId="2" r:id="rId2"/>
     <sheet name="UserManagement" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>1</t>
   </si>
@@ -107,25 +107,19 @@
     <t>Id</t>
   </si>
   <si>
+    <t>P@ssw0rd1!</t>
+  </si>
+  <si>
+    <t>marco.lobo@janeirodigital.com</t>
+  </si>
+  <si>
     <t>Tenant 2 Desc</t>
-  </si>
-  <si>
-    <t>Cesar</t>
-  </si>
-  <si>
-    <t>Gonzalez</t>
-  </si>
-  <si>
-    <t>P@ssw0rd1!</t>
-  </si>
-  <si>
-    <t>marco.lobo@janeirodigital.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -170,7 +164,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -448,14 +442,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" bestFit="1" customWidth="1"/>
@@ -497,9 +491,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{6C2BBAD7-587D-4AD1-A1EA-997B20EA2D27}"/>
-    <hyperlink ref="C1" r:id="rId2" xr:uid="{741B009E-B31E-44B1-9481-2F2C06029C57}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{90FD050E-CC8B-490D-9F4C-A843C35B4F5D}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C1" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -507,14 +501,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
@@ -548,9 +542,9 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -559,34 +553,35 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="C1" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{426BF298-3202-426D-BE0D-F144A4E9CDB5}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{EFC4F137-F318-41B3-8A8F-BB3A079FF4D1}"/>
-    <hyperlink ref="B4" r:id="rId5" xr:uid="{F4B219D8-65D3-4FBC-8335-A2F14B899918}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C1" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="C3" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC247988-D3D6-4F67-B060-1E538F8A4EB7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
@@ -691,7 +686,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
@@ -700,10 +695,10 @@
         <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>25</v>
@@ -729,10 +724,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{7850A4E8-B209-4700-9C70-F537F104F067}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{D59C0627-7585-43C9-94B2-E22B99623013}"/>
-    <hyperlink ref="H3" r:id="rId3" xr:uid="{0194950A-60E5-4F5A-9D4B-1A86DD9A4D42}"/>
-    <hyperlink ref="I3" r:id="rId4" xr:uid="{1C0B9623-DAE1-415F-8DB8-2EC701AAE334}"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId2"/>
+    <hyperlink ref="H3" r:id="rId3"/>
+    <hyperlink ref="I3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
(SVBF-162) - QA - After code review feedback - depend on SVBF-133 - QA - After code review feedback
Signed-off-by: julio-oropeza-jd <julio.oropeza@janeirodigital.com>
</commit_message>
<xml_diff>
--- a/xform-automation-webdriver/controllers/src/main/resources/ParameterFile.xlsx
+++ b/xform-automation-webdriver/controllers/src/main/resources/ParameterFile.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Profiles" sheetId="1" r:id="rId1"/>
-    <sheet name="Parameters" sheetId="2" r:id="rId2"/>
-    <sheet name="UserManagement" sheetId="3" r:id="rId3"/>
+    <sheet name="0_Profiles" sheetId="1" r:id="rId1"/>
+    <sheet name="1_Parameters" sheetId="2" r:id="rId2"/>
+    <sheet name="2_UserManagement" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -164,7 +164,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -442,14 +442,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" bestFit="1" customWidth="1"/>
@@ -491,9 +491,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C1" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C1" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -501,14 +501,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
@@ -561,12 +561,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C1" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="C4" r:id="rId4"/>
-    <hyperlink ref="B4" r:id="rId5"/>
-    <hyperlink ref="C3" r:id="rId6"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C1" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="C3" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
@@ -574,14 +574,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
@@ -724,10 +724,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="I2" r:id="rId2"/>
-    <hyperlink ref="H3" r:id="rId3"/>
-    <hyperlink ref="I3" r:id="rId4"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="I3" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
(XF-518) - QA - Demo Web Driver - Feature to allow multiple XForm related projects
Signed-off-by: julio-oropeza-jd <julio.oropeza@janeirodigital.com>
</commit_message>
<xml_diff>
--- a/xform-automation-webdriver/controllers/src/main/resources/ParameterFile.xlsx
+++ b/xform-automation-webdriver/controllers/src/main/resources/ParameterFile.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0_Profiles" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t>1</t>
   </si>
@@ -114,6 +114,18 @@
   </si>
   <si>
     <t>Tenant 2 Desc</t>
+  </si>
+  <si>
+    <t>SVB Founders Platform</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>xxx@janeirodigital.com</t>
+  </si>
+  <si>
+    <t>zzz@janeirodigital.com</t>
   </si>
 </sst>
 </file>
@@ -445,7 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -577,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,16 +675,16 @@
         <v>25</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>19</v>
@@ -704,16 +716,16 @@
         <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
(XF-567) - QA - TC Read navigation flow - Validations of the navigation flow - Add new user (in progress) - Redis Injection fuctionality
Signed-off-by: julio-oropeza-jd <julio.oropeza@janeirodigital.com>
</commit_message>
<xml_diff>
--- a/xform-automation-webdriver/controllers/src/main/resources/ParameterFile.xlsx
+++ b/xform-automation-webdriver/controllers/src/main/resources/ParameterFile.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4CDF16-CA35-4B59-A10D-C32CF119CCC3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10,6 +11,9 @@
     <sheet name="0_Profiles" sheetId="1" r:id="rId1"/>
     <sheet name="1_Parameters" sheetId="2" r:id="rId2"/>
     <sheet name="2_UserManagement" sheetId="3" r:id="rId3"/>
+    <sheet name="3_TenantsManagement" sheetId="5" r:id="rId4"/>
+    <sheet name="4_SystemAdmManagement" sheetId="6" r:id="rId5"/>
+    <sheet name="5_RedisHistories_Insertion" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
   <si>
     <t>1</t>
   </si>
@@ -116,9 +120,6 @@
     <t>Tenant 2 Desc</t>
   </si>
   <si>
-    <t>SVB Founders Platform</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
@@ -126,6 +127,39 @@
   </si>
   <si>
     <t>zzz@janeirodigital.com</t>
+  </si>
+  <si>
+    <t>marcos.zapata@janeirodigital.com</t>
+  </si>
+  <si>
+    <t>Server_Id</t>
+  </si>
+  <si>
+    <t>Unix_TimeStamp</t>
+  </si>
+  <si>
+    <t>Current_Value</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>20180418001122</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>321</t>
+  </si>
+  <si>
+    <t>20180417332211</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>RowActive</t>
   </si>
 </sst>
 </file>
@@ -514,10 +548,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,53 +569,65 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>29</v>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="C1" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="B4" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="C3" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{9A9A03B6-7FE0-439A-B554-D869439CB2A5}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{E7EFF001-3064-41D8-9954-144BAB004939}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -589,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,16 +721,16 @@
         <v>25</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>19</v>
@@ -716,16 +762,16 @@
         <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>19</v>
@@ -744,4 +790,92 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C794124D-C84F-445E-8926-80FD211F1A89}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A0180E-38C0-478D-8855-979B1B5E5844}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CBE87E-0013-470B-8F63-B77A58369D23}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
(XF-875) - Automation script for user creation. - Add a click in close button for the notification banner - Add getRandomValue method in utils class - Add emailGenerator method - Add random value in the domains for email address - Create Script 7 User management class - Create and testNG xml for User Management Section - Include date time in the email generator method
Signed-off-by: Gerardo Soto <gerardo.soto@janeirodigital.com>
</commit_message>
<xml_diff>
--- a/xform-automation-webdriver/controllers/src/main/resources/ParameterFile.xlsx
+++ b/xform-automation-webdriver/controllers/src/main/resources/ParameterFile.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4CDF16-CA35-4B59-A10D-C32CF119CCC3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1F9B61-2AA7-914D-B9AC-97BB860C219A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24360" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0_Profiles" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
   <si>
     <t>1</t>
   </si>
@@ -117,18 +117,12 @@
     <t>marco.lobo@janeirodigital.com</t>
   </si>
   <si>
-    <t>Tenant 2 Desc</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
     <t>xxx@janeirodigital.com</t>
   </si>
   <si>
-    <t>zzz@janeirodigital.com</t>
-  </si>
-  <si>
     <t>marcos.zapata@janeirodigital.com</t>
   </si>
   <si>
@@ -160,6 +154,15 @@
   </si>
   <si>
     <t>RowActive</t>
+  </si>
+  <si>
+    <t>Gerardo</t>
+  </si>
+  <si>
+    <t>Soto</t>
+  </si>
+  <si>
+    <t>ger@janeirodigital.com</t>
   </si>
 </sst>
 </file>
@@ -495,14 +498,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,7 +516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -524,7 +527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -554,14 +557,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -572,7 +575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -583,7 +586,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -594,7 +597,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -605,7 +608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -613,7 +616,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -636,28 +639,28 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
     <col min="2" max="2" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -698,7 +701,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -712,22 +715,22 @@
         <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>18</v>
@@ -739,12 +742,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>19</v>
@@ -762,16 +765,16 @@
         <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>19</v>
@@ -782,10 +785,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="H3" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="I3" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="H2" r:id="rId3" xr:uid="{DCCC1DEE-B5C3-344C-B037-E03AB1466A99}"/>
+    <hyperlink ref="I2" r:id="rId4" xr:uid="{78699318-E936-D34E-8464-5C31734DD30D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -798,7 +801,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -810,7 +813,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -824,55 +827,55 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(XF-876) AUTO_TC 7.3.3 Update User Data - UpdateUser Method - Scroll Methods - getListOfElement Method - Getting data from the excel.xlsx
Signed-off-by: Gerardo Soto <gerardo.soto@janeirodigital.com>
</commit_message>
<xml_diff>
--- a/xform-automation-webdriver/controllers/src/main/resources/ParameterFile.xlsx
+++ b/xform-automation-webdriver/controllers/src/main/resources/ParameterFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1F9B61-2AA7-914D-B9AC-97BB860C219A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEC519A-3E8F-F04F-9319-2697048E69D8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24360" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
   <si>
     <t>1</t>
   </si>
@@ -96,9 +96,6 @@
     <t>none</t>
   </si>
   <si>
-    <t>Julio</t>
-  </si>
-  <si>
     <t>Oropeza</t>
   </si>
   <si>
@@ -156,13 +153,22 @@
     <t>RowActive</t>
   </si>
   <si>
-    <t>Gerardo</t>
-  </si>
-  <si>
     <t>Soto</t>
   </si>
   <si>
     <t>ger@janeirodigital.com</t>
+  </si>
+  <si>
+    <t>tGerardo</t>
+  </si>
+  <si>
+    <t>tJulio</t>
+  </si>
+  <si>
+    <t>Job Title Change</t>
+  </si>
+  <si>
+    <t>Test Job Title</t>
   </si>
 </sst>
 </file>
@@ -580,10 +586,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -591,10 +597,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -616,7 +622,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -636,10 +642,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -660,9 +666,9 @@
     <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -700,8 +706,11 @@
       <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -715,22 +724,22 @@
         <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>18</v>
@@ -741,8 +750,11 @@
       <c r="M2" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -756,22 +768,22 @@
         <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>18</v>
@@ -781,6 +793,9 @@
       </c>
       <c r="M3" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -838,16 +853,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -855,13 +870,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -869,13 +884,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(XF-877) Internal - AUTO_TC 7.2.1 Read listed info from User - Update for UpdateUser Method (getting data from the excel file) - UserRead method creation - TestNG dependencies between @Test for User Management CRUD. - PR Changes
Signed-off-by: Gerardo Soto <gerardo.soto@janeirodigital.com>
</commit_message>
<xml_diff>
--- a/xform-automation-webdriver/controllers/src/main/resources/ParameterFile.xlsx
+++ b/xform-automation-webdriver/controllers/src/main/resources/ParameterFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEC519A-3E8F-F04F-9319-2697048E69D8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A35F369-2161-034D-84F8-B553891683FA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="24360" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
   <si>
     <t>1</t>
   </si>
@@ -96,79 +96,97 @@
     <t>none</t>
   </si>
   <si>
+    <t>Qa Tester</t>
+  </si>
+  <si>
+    <t>julio.oropeza@janeirodigital.com</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>P@ssw0rd1!</t>
+  </si>
+  <si>
+    <t>marco.lobo@janeirodigital.com</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>xxx@janeirodigital.com</t>
+  </si>
+  <si>
+    <t>marcos.zapata@janeirodigital.com</t>
+  </si>
+  <si>
+    <t>Server_Id</t>
+  </si>
+  <si>
+    <t>Unix_TimeStamp</t>
+  </si>
+  <si>
+    <t>Current_Value</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>20180418001122</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>321</t>
+  </si>
+  <si>
+    <t>20180417332211</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>RowActive</t>
+  </si>
+  <si>
+    <t>ger@janeirodigital.com</t>
+  </si>
+  <si>
+    <t>tGerardo</t>
+  </si>
+  <si>
+    <t>tJulio</t>
+  </si>
+  <si>
+    <t>Job Title Change</t>
+  </si>
+  <si>
+    <t>Test Job Title</t>
+  </si>
+  <si>
+    <t>NameChange</t>
+  </si>
+  <si>
+    <t>Last Name Change</t>
+  </si>
+  <si>
+    <t>tGerardoC</t>
+  </si>
+  <si>
+    <t>tJulioC</t>
+  </si>
+  <si>
+    <t>Soto</t>
+  </si>
+  <si>
     <t>Oropeza</t>
   </si>
   <si>
-    <t>Qa Tester</t>
-  </si>
-  <si>
-    <t>julio.oropeza@janeirodigital.com</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>P@ssw0rd1!</t>
-  </si>
-  <si>
-    <t>marco.lobo@janeirodigital.com</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>xxx@janeirodigital.com</t>
-  </si>
-  <si>
-    <t>marcos.zapata@janeirodigital.com</t>
-  </si>
-  <si>
-    <t>Server_Id</t>
-  </si>
-  <si>
-    <t>Unix_TimeStamp</t>
-  </si>
-  <si>
-    <t>Current_Value</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>20180418001122</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>321</t>
-  </si>
-  <si>
-    <t>20180417332211</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>RowActive</t>
-  </si>
-  <si>
-    <t>Soto</t>
-  </si>
-  <si>
-    <t>ger@janeirodigital.com</t>
-  </si>
-  <si>
-    <t>tGerardo</t>
-  </si>
-  <si>
-    <t>tJulio</t>
-  </si>
-  <si>
-    <t>Job Title Change</t>
-  </si>
-  <si>
-    <t>Test Job Title</t>
+    <t>SotoC</t>
+  </si>
+  <si>
+    <t>OropezaC</t>
   </si>
 </sst>
 </file>
@@ -586,10 +604,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -597,10 +615,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -622,7 +640,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -642,10 +660,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -666,9 +684,9 @@
     <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -707,10 +725,16 @@
         <v>20</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -724,22 +748,22 @@
         <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>18</v>
@@ -751,10 +775,16 @@
         <v>21</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -768,22 +798,22 @@
         <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>18</v>
@@ -795,7 +825,13 @@
         <v>21</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -853,16 +889,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -870,13 +906,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -884,13 +920,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>